<commit_message>
faster calculation in roller coaster model
</commit_message>
<xml_diff>
--- a/Model_TopSim_RollerCoaster/RollerCoaster_Model_Definition.xlsx
+++ b/Model_TopSim_RollerCoaster/RollerCoaster_Model_Definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malteebner/Library/Mobile Documents/com~apple~CloudDocs/Master ETIT/10. Semester/Forschungsarbeit/Code Forschungsarbeit/Model_TopSim_RollerCoaster/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20828310-54E3-9C4D-B59A-0090486618B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB548049-4167-504E-92D0-EA514D70D6BD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{FCED99B0-49FF-5541-B4A0-4C6030238B64}"/>
   </bookViews>
@@ -272,12 +272,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -292,8 +298,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,36 +615,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A15AD41-7732-DC45-B8B2-B8C789AA2988}">
-  <dimension ref="A1:AN49"/>
+  <dimension ref="A1:AR49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="1.33203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="2.5" style="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>0</v>
       </c>
@@ -650,130 +664,130 @@
       <c r="D1">
         <v>3</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>4</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <v>5</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <v>6</v>
       </c>
-      <c r="H1">
+      <c r="I1">
         <v>7</v>
       </c>
-      <c r="I1">
+      <c r="J1">
         <v>8</v>
       </c>
-      <c r="J1">
+      <c r="L1">
         <v>9</v>
       </c>
-      <c r="K1">
+      <c r="M1">
         <v>10</v>
       </c>
-      <c r="L1">
+      <c r="N1">
         <v>11</v>
       </c>
-      <c r="M1">
+      <c r="O1">
         <v>12</v>
       </c>
-      <c r="N1">
+      <c r="P1">
         <v>13</v>
       </c>
-      <c r="O1">
+      <c r="R1">
         <v>14</v>
       </c>
-      <c r="P1">
+      <c r="S1">
         <v>15</v>
       </c>
-      <c r="Q1">
+      <c r="T1">
         <v>16</v>
       </c>
-      <c r="R1">
+      <c r="U1">
         <v>17</v>
       </c>
-      <c r="S1">
+      <c r="V1">
         <v>18</v>
       </c>
-      <c r="T1">
+      <c r="X1">
         <v>19</v>
       </c>
-      <c r="U1">
+      <c r="Y1">
         <v>20</v>
       </c>
-      <c r="V1">
+      <c r="Z1">
         <v>21</v>
       </c>
-      <c r="W1">
+      <c r="AA1">
         <v>22</v>
       </c>
-      <c r="X1">
+      <c r="AB1">
         <v>23</v>
       </c>
-      <c r="Y1">
+      <c r="AC1">
         <v>24</v>
       </c>
-      <c r="Z1">
+      <c r="AD1">
         <v>25</v>
       </c>
-      <c r="AA1">
+      <c r="AE1">
         <v>26</v>
       </c>
-      <c r="AB1">
+      <c r="AF1">
         <v>27</v>
       </c>
-      <c r="AC1">
+      <c r="AG1">
         <v>28</v>
       </c>
-      <c r="AD1">
+      <c r="AH1">
         <v>29</v>
       </c>
-      <c r="AE1">
+      <c r="AI1">
         <v>30</v>
       </c>
-      <c r="AF1">
+      <c r="AJ1">
         <v>31</v>
       </c>
-      <c r="AG1">
+      <c r="AK1">
         <v>32</v>
       </c>
-      <c r="AH1">
+      <c r="AL1">
         <v>33</v>
       </c>
-      <c r="AI1">
+      <c r="AM1">
         <v>34</v>
       </c>
-      <c r="AJ1">
+      <c r="AN1">
         <v>35</v>
       </c>
-      <c r="AK1">
+      <c r="AO1">
         <v>36</v>
       </c>
-      <c r="AL1">
+      <c r="AP1">
         <v>37</v>
       </c>
-      <c r="AM1">
+      <c r="AQ1">
         <v>38</v>
       </c>
-      <c r="AN1">
+      <c r="AR1">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="E2" t="s">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>8</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" t="s">
         <v>9</v>
       </c>
-      <c r="T2" t="s">
+      <c r="X2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -783,68 +797,68 @@
       <c r="D3" t="s">
         <v>55</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>73</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>74</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>2</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>3</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>6</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>73</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>74</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>2</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>3</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
         <v>6</v>
       </c>
-      <c r="O3" t="s">
+      <c r="R3" t="s">
         <v>73</v>
       </c>
-      <c r="P3" t="s">
+      <c r="S3" t="s">
         <v>74</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="T3" t="s">
         <v>2</v>
       </c>
-      <c r="R3" t="s">
+      <c r="U3" t="s">
         <v>3</v>
       </c>
-      <c r="S3" t="s">
+      <c r="V3" t="s">
         <v>6</v>
       </c>
-      <c r="T3" t="s">
+      <c r="X3" t="s">
         <v>73</v>
       </c>
-      <c r="U3" t="s">
+      <c r="Y3" t="s">
         <v>74</v>
       </c>
-      <c r="V3" t="s">
+      <c r="Z3" t="s">
         <v>2</v>
       </c>
-      <c r="W3" t="s">
+      <c r="AA3" t="s">
         <v>3</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AB3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>1</v>
       </c>
@@ -854,136 +868,136 @@
       <c r="D4" t="s">
         <v>56</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>8</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>210</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
         <v>0.1</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>6</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>320</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>-1</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>-1</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>0.2</v>
       </c>
-      <c r="O4">
+      <c r="R4">
         <v>5</v>
       </c>
-      <c r="P4">
+      <c r="S4">
         <v>380</v>
       </c>
-      <c r="Q4">
+      <c r="T4">
         <v>-2</v>
       </c>
-      <c r="R4">
+      <c r="U4">
         <v>-2</v>
       </c>
-      <c r="S4">
+      <c r="V4">
         <v>0.4</v>
       </c>
-      <c r="T4">
+      <c r="X4">
         <v>10</v>
       </c>
-      <c r="U4">
+      <c r="Y4">
         <v>190</v>
       </c>
-      <c r="V4">
+      <c r="Z4">
         <v>1</v>
       </c>
-      <c r="W4">
+      <c r="AA4">
         <v>1</v>
       </c>
-      <c r="X4">
+      <c r="AB4">
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>65</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>400</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
         <v>0.1</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>40</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>430</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>1</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>1</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>0.2</v>
       </c>
-      <c r="O5">
+      <c r="R5">
         <v>40</v>
       </c>
-      <c r="P5">
+      <c r="S5">
         <v>450</v>
       </c>
-      <c r="Q5">
+      <c r="T5">
         <v>2</v>
       </c>
-      <c r="R5">
+      <c r="U5">
         <v>2</v>
       </c>
-      <c r="S5">
+      <c r="V5">
         <v>0.4</v>
       </c>
-      <c r="T5">
+      <c r="X5">
         <v>40</v>
       </c>
-      <c r="U5">
+      <c r="Y5">
         <v>500</v>
       </c>
-      <c r="V5">
+      <c r="Z5">
         <v>2</v>
       </c>
-      <c r="W5">
+      <c r="AA5">
         <v>1</v>
       </c>
-      <c r="X5">
+      <c r="AB5">
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>3</v>
       </c>
@@ -993,68 +1007,68 @@
       <c r="D6" t="s">
         <v>57</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>7</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>130</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
         <v>0.1</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>6</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <v>150</v>
       </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
       <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
         <v>0.2</v>
       </c>
-      <c r="O6">
+      <c r="R6">
         <v>5</v>
       </c>
-      <c r="P6">
+      <c r="S6">
         <v>190</v>
       </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
         <v>0.4</v>
       </c>
-      <c r="T6">
+      <c r="X6">
         <v>9</v>
       </c>
-      <c r="U6">
+      <c r="Y6">
         <v>110</v>
       </c>
-      <c r="V6">
+      <c r="Z6">
         <v>1</v>
       </c>
-      <c r="W6">
+      <c r="AA6">
         <v>1</v>
       </c>
-      <c r="X6">
+      <c r="AB6">
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>4</v>
       </c>
@@ -1064,68 +1078,68 @@
       <c r="D7" t="s">
         <v>58</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>6</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>90</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
         <v>0.1</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>5</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>140</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>-1</v>
       </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
         <v>0.2</v>
       </c>
-      <c r="O7">
+      <c r="R7">
         <v>4</v>
       </c>
-      <c r="P7">
+      <c r="S7">
         <v>170</v>
       </c>
-      <c r="Q7">
+      <c r="T7">
         <v>-1</v>
       </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
         <v>0.4</v>
       </c>
-      <c r="T7">
+      <c r="X7">
         <v>7</v>
       </c>
-      <c r="U7">
-        <v>100</v>
-      </c>
-      <c r="V7">
+      <c r="Y7">
+        <v>100</v>
+      </c>
+      <c r="Z7">
         <v>1</v>
       </c>
-      <c r="W7">
+      <c r="AA7">
         <v>1</v>
       </c>
-      <c r="X7">
+      <c r="AB7">
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>5</v>
       </c>
@@ -1135,68 +1149,68 @@
       <c r="D8" t="s">
         <v>59</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>7</v>
       </c>
-      <c r="F8">
-        <v>120</v>
-      </c>
       <c r="G8">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
         <v>0.1</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>6</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>170</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <v>-1</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>-1</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>0.2</v>
       </c>
-      <c r="O8">
+      <c r="R8">
         <v>4</v>
       </c>
-      <c r="P8">
+      <c r="S8">
         <v>210</v>
       </c>
-      <c r="Q8">
+      <c r="T8">
         <v>-1</v>
       </c>
-      <c r="R8">
+      <c r="U8">
         <v>-2</v>
       </c>
-      <c r="S8">
+      <c r="V8">
         <v>0.4</v>
       </c>
-      <c r="T8">
+      <c r="X8">
         <v>8</v>
       </c>
-      <c r="U8">
-        <v>120</v>
-      </c>
-      <c r="V8">
+      <c r="Y8">
+        <v>120</v>
+      </c>
+      <c r="Z8">
         <v>2</v>
       </c>
-      <c r="W8">
+      <c r="AA8">
         <v>1</v>
       </c>
-      <c r="X8">
+      <c r="AB8">
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>6</v>
       </c>
@@ -1206,68 +1220,68 @@
       <c r="D9" t="s">
         <v>60</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>5</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>80</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
         <v>0.1</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>5</v>
       </c>
-      <c r="K9">
-        <v>100</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
       <c r="M9">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
         <v>0.2</v>
       </c>
-      <c r="O9">
+      <c r="R9">
         <v>4</v>
       </c>
-      <c r="P9">
+      <c r="S9">
         <v>140</v>
       </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
         <v>0.4</v>
       </c>
-      <c r="T9">
+      <c r="X9">
         <v>7</v>
       </c>
-      <c r="U9">
+      <c r="Y9">
         <v>70</v>
       </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
-      <c r="W9">
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
         <v>1</v>
       </c>
-      <c r="X9">
+      <c r="AB9">
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>7</v>
       </c>
@@ -1277,68 +1291,68 @@
       <c r="D10">
         <v>11</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>3</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>90</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
         <v>0.1</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>2</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>130</v>
       </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
       <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
         <v>0.2</v>
       </c>
-      <c r="O10">
+      <c r="R10">
         <v>1</v>
       </c>
-      <c r="P10">
+      <c r="S10">
         <v>190</v>
       </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
         <v>0.4</v>
       </c>
-      <c r="T10">
+      <c r="X10">
         <v>5</v>
       </c>
-      <c r="U10">
+      <c r="Y10">
         <v>80</v>
       </c>
-      <c r="V10">
-        <v>0</v>
-      </c>
-      <c r="W10">
-        <v>0</v>
-      </c>
-      <c r="X10">
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>8</v>
       </c>
@@ -1348,68 +1362,68 @@
       <c r="D11">
         <v>20</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>4</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>180</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
         <v>0.1</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>3</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>240</v>
       </c>
-      <c r="L11">
+      <c r="N11">
         <v>-1</v>
       </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
         <v>0.2</v>
       </c>
-      <c r="O11">
+      <c r="R11">
         <v>2</v>
       </c>
-      <c r="P11">
+      <c r="S11">
         <v>400</v>
       </c>
-      <c r="Q11">
+      <c r="T11">
         <v>-1</v>
       </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
         <v>0.4</v>
       </c>
-      <c r="T11">
+      <c r="X11">
         <v>5</v>
       </c>
-      <c r="U11">
+      <c r="Y11">
         <v>160</v>
       </c>
-      <c r="V11">
+      <c r="Z11">
         <v>1</v>
       </c>
-      <c r="W11">
+      <c r="AA11">
         <v>1</v>
       </c>
-      <c r="X11">
+      <c r="AB11">
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>9</v>
       </c>
@@ -1419,68 +1433,68 @@
       <c r="D12">
         <v>14</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>6</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>40</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
         <v>0.1</v>
       </c>
-      <c r="J12">
+      <c r="L12">
         <v>5</v>
       </c>
-      <c r="K12">
+      <c r="M12">
         <v>60</v>
       </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
       <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
         <v>0.2</v>
       </c>
-      <c r="O12">
+      <c r="R12">
         <v>4</v>
       </c>
-      <c r="P12">
+      <c r="S12">
         <v>70</v>
       </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
-      <c r="S12">
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
         <v>0.4</v>
       </c>
-      <c r="T12">
+      <c r="X12">
         <v>8</v>
       </c>
-      <c r="U12">
+      <c r="Y12">
         <v>40</v>
       </c>
-      <c r="V12">
-        <v>0</v>
-      </c>
-      <c r="W12">
-        <v>0</v>
-      </c>
-      <c r="X12">
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>10</v>
       </c>
@@ -1490,68 +1504,68 @@
       <c r="D13">
         <v>22</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>8</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>240</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
         <v>0.1</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <v>8</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <v>300</v>
       </c>
-      <c r="L13">
+      <c r="N13">
         <v>2</v>
       </c>
-      <c r="M13">
+      <c r="O13">
         <v>1</v>
       </c>
-      <c r="N13">
+      <c r="P13">
         <v>0.2</v>
       </c>
-      <c r="O13">
+      <c r="R13">
         <v>6</v>
       </c>
-      <c r="P13">
+      <c r="S13">
         <v>380</v>
       </c>
-      <c r="Q13">
+      <c r="T13">
         <v>-2</v>
       </c>
-      <c r="R13">
+      <c r="U13">
         <v>-2</v>
       </c>
-      <c r="S13">
+      <c r="V13">
         <v>0.4</v>
       </c>
-      <c r="T13">
+      <c r="X13">
         <v>9</v>
       </c>
-      <c r="U13">
+      <c r="Y13">
         <v>320</v>
       </c>
-      <c r="V13">
+      <c r="Z13">
         <v>2</v>
       </c>
-      <c r="W13">
+      <c r="AA13">
         <v>1</v>
       </c>
-      <c r="X13">
+      <c r="AB13">
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>11</v>
       </c>
@@ -1561,68 +1575,68 @@
       <c r="D14">
         <v>15</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>4</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>260</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
         <v>0.1</v>
       </c>
-      <c r="J14">
+      <c r="L14">
         <v>3</v>
       </c>
-      <c r="K14">
+      <c r="M14">
         <v>310</v>
       </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
       <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
         <v>0.2</v>
       </c>
-      <c r="O14">
+      <c r="R14">
         <v>2</v>
       </c>
-      <c r="P14">
+      <c r="S14">
         <v>390</v>
       </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
-      <c r="S14">
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
         <v>0.4</v>
       </c>
-      <c r="T14">
+      <c r="X14">
         <v>6</v>
       </c>
-      <c r="U14">
+      <c r="Y14">
         <v>220</v>
       </c>
-      <c r="V14">
-        <v>0</v>
-      </c>
-      <c r="W14">
-        <v>0</v>
-      </c>
-      <c r="X14">
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>12</v>
       </c>
@@ -1632,68 +1646,68 @@
       <c r="D15">
         <v>17</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>5</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>90</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
         <v>0.1</v>
       </c>
-      <c r="J15">
+      <c r="L15">
         <v>4</v>
       </c>
-      <c r="K15">
+      <c r="M15">
         <v>140</v>
       </c>
-      <c r="L15">
+      <c r="N15">
         <v>-1</v>
       </c>
-      <c r="M15">
+      <c r="O15">
         <v>-1</v>
       </c>
-      <c r="N15">
+      <c r="P15">
         <v>0.2</v>
       </c>
-      <c r="O15">
+      <c r="R15">
         <v>3</v>
       </c>
-      <c r="P15">
+      <c r="S15">
         <v>190</v>
       </c>
-      <c r="Q15">
+      <c r="T15">
         <v>-1</v>
       </c>
-      <c r="R15">
+      <c r="U15">
         <v>-1</v>
       </c>
-      <c r="S15">
+      <c r="V15">
         <v>0.4</v>
       </c>
-      <c r="T15">
+      <c r="X15">
         <v>7</v>
       </c>
-      <c r="U15">
+      <c r="Y15">
         <v>90</v>
       </c>
-      <c r="V15">
+      <c r="Z15">
         <v>1</v>
       </c>
-      <c r="W15">
+      <c r="AA15">
         <v>1</v>
       </c>
-      <c r="X15">
+      <c r="AB15">
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>13</v>
       </c>
@@ -1703,68 +1717,68 @@
       <c r="D16">
         <v>18</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>6</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>70</v>
       </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
         <v>0.1</v>
       </c>
-      <c r="J16">
+      <c r="L16">
         <v>5</v>
       </c>
-      <c r="K16">
-        <v>120</v>
-      </c>
-      <c r="L16">
+      <c r="M16">
+        <v>120</v>
+      </c>
+      <c r="N16">
         <v>-2</v>
       </c>
-      <c r="M16">
+      <c r="O16">
         <v>-1</v>
       </c>
-      <c r="N16">
+      <c r="P16">
         <v>0.2</v>
       </c>
-      <c r="O16">
+      <c r="R16">
         <v>3</v>
       </c>
-      <c r="P16">
+      <c r="S16">
         <v>160</v>
       </c>
-      <c r="Q16">
+      <c r="T16">
         <v>-2</v>
       </c>
-      <c r="R16">
+      <c r="U16">
         <v>-1</v>
       </c>
-      <c r="S16">
+      <c r="V16">
         <v>0.4</v>
       </c>
-      <c r="T16">
+      <c r="X16">
         <v>8</v>
       </c>
-      <c r="U16">
+      <c r="Y16">
         <v>80</v>
       </c>
-      <c r="V16">
+      <c r="Z16">
         <v>2</v>
       </c>
-      <c r="W16">
+      <c r="AA16">
         <v>2</v>
       </c>
-      <c r="X16">
+      <c r="AB16">
         <v>0.01</v>
       </c>
     </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>14</v>
       </c>
@@ -1774,68 +1788,68 @@
       <c r="D17">
         <v>21</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>21</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>270</v>
       </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
         <v>0.1</v>
       </c>
-      <c r="J17">
+      <c r="L17">
         <v>18</v>
       </c>
-      <c r="K17">
+      <c r="M17">
         <v>340</v>
       </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
       <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
         <v>0.2</v>
       </c>
-      <c r="O17">
+      <c r="R17">
         <v>16</v>
       </c>
-      <c r="P17">
+      <c r="S17">
         <v>410</v>
       </c>
-      <c r="Q17">
+      <c r="T17">
         <v>-1</v>
       </c>
-      <c r="R17">
-        <v>0</v>
-      </c>
-      <c r="S17">
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
         <v>0.4</v>
       </c>
-      <c r="T17">
+      <c r="X17">
         <v>24</v>
       </c>
-      <c r="U17">
+      <c r="Y17">
         <v>260</v>
       </c>
-      <c r="V17">
+      <c r="Z17">
         <v>1</v>
       </c>
-      <c r="W17">
-        <v>0</v>
-      </c>
-      <c r="X17">
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17">
         <v>0.01</v>
       </c>
     </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>15</v>
       </c>
@@ -1845,68 +1859,68 @@
       <c r="D18">
         <v>23</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>8</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>380</v>
       </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
         <v>0.1</v>
       </c>
-      <c r="J18">
+      <c r="L18">
         <v>7</v>
       </c>
-      <c r="K18">
+      <c r="M18">
         <v>420</v>
       </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
         <v>-1</v>
       </c>
-      <c r="N18">
+      <c r="P18">
         <v>0.2</v>
       </c>
-      <c r="O18">
+      <c r="R18">
         <v>5</v>
       </c>
-      <c r="P18">
+      <c r="S18">
         <v>490</v>
       </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
         <v>-2</v>
       </c>
-      <c r="S18">
+      <c r="V18">
         <v>0.4</v>
       </c>
-      <c r="T18">
+      <c r="X18">
         <v>10</v>
       </c>
-      <c r="U18">
+      <c r="Y18">
         <v>360</v>
       </c>
-      <c r="V18">
-        <v>0</v>
-      </c>
-      <c r="W18">
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18">
         <v>2</v>
       </c>
-      <c r="X18">
+      <c r="AB18">
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>16</v>
       </c>
@@ -1916,68 +1930,68 @@
       <c r="D19">
         <v>24</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>18</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>1100</v>
       </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
         <v>0.1</v>
       </c>
-      <c r="J19">
+      <c r="L19">
         <v>16</v>
       </c>
-      <c r="K19">
+      <c r="M19">
         <v>1250</v>
       </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
         <v>-2</v>
       </c>
-      <c r="N19">
+      <c r="P19">
         <v>0.2</v>
       </c>
-      <c r="O19">
+      <c r="R19">
         <v>12</v>
       </c>
-      <c r="P19">
+      <c r="S19">
         <v>1350</v>
       </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19">
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
         <v>-2</v>
       </c>
-      <c r="S19">
+      <c r="V19">
         <v>0.4</v>
       </c>
-      <c r="T19">
+      <c r="X19">
         <v>22</v>
       </c>
-      <c r="U19">
+      <c r="Y19">
         <v>950</v>
       </c>
-      <c r="V19">
-        <v>0</v>
-      </c>
-      <c r="W19">
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
         <v>2</v>
       </c>
-      <c r="X19">
+      <c r="AB19">
         <v>0.01</v>
       </c>
     </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>17</v>
       </c>
@@ -1987,68 +2001,68 @@
       <c r="D20">
         <v>26</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>16</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>900</v>
       </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
         <v>0.1</v>
       </c>
-      <c r="J20">
+      <c r="L20">
         <v>15</v>
       </c>
-      <c r="K20">
+      <c r="M20">
         <v>950</v>
       </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
       <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
         <v>0.2</v>
       </c>
-      <c r="O20">
+      <c r="R20">
         <v>12</v>
       </c>
-      <c r="P20">
+      <c r="S20">
         <v>1000</v>
       </c>
-      <c r="Q20">
+      <c r="T20">
         <v>-2</v>
       </c>
-      <c r="R20">
+      <c r="U20">
         <v>-2</v>
       </c>
-      <c r="S20">
+      <c r="V20">
         <v>0.4</v>
       </c>
-      <c r="T20">
+      <c r="X20">
         <v>18</v>
       </c>
-      <c r="U20">
+      <c r="Y20">
         <v>820</v>
       </c>
-      <c r="V20">
+      <c r="Z20">
         <v>2</v>
       </c>
-      <c r="W20">
+      <c r="AA20">
         <v>1</v>
       </c>
-      <c r="X20">
+      <c r="AB20">
         <v>0.01</v>
       </c>
     </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>18</v>
       </c>
@@ -2058,68 +2072,68 @@
       <c r="D21">
         <v>27</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>17</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>280</v>
       </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
         <v>0.1</v>
       </c>
-      <c r="J21">
+      <c r="L21">
         <v>15</v>
       </c>
-      <c r="K21">
+      <c r="M21">
         <v>390</v>
       </c>
-      <c r="L21">
+      <c r="N21">
         <v>-2</v>
       </c>
-      <c r="M21">
+      <c r="O21">
         <v>-1</v>
       </c>
-      <c r="N21">
+      <c r="P21">
         <v>0.2</v>
       </c>
-      <c r="O21">
+      <c r="R21">
         <v>13</v>
       </c>
-      <c r="P21">
+      <c r="S21">
         <v>430</v>
       </c>
-      <c r="Q21">
+      <c r="T21">
         <v>-3</v>
       </c>
-      <c r="R21">
+      <c r="U21">
         <v>-3</v>
       </c>
-      <c r="S21">
+      <c r="V21">
         <v>0.4</v>
       </c>
-      <c r="T21">
+      <c r="X21">
         <v>19</v>
       </c>
-      <c r="U21">
+      <c r="Y21">
         <v>300</v>
       </c>
-      <c r="V21">
+      <c r="Z21">
         <v>2</v>
       </c>
-      <c r="W21">
+      <c r="AA21">
         <v>1</v>
       </c>
-      <c r="X21">
+      <c r="AB21">
         <v>0.01</v>
       </c>
     </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>19</v>
       </c>
@@ -2129,68 +2143,68 @@
       <c r="D22" t="s">
         <v>61</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>8</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>160</v>
       </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
       <c r="H22">
         <v>0</v>
       </c>
       <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
         <v>0.1</v>
       </c>
-      <c r="J22">
+      <c r="L22">
         <v>7</v>
       </c>
-      <c r="K22">
+      <c r="M22">
         <v>190</v>
       </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
         <v>-1</v>
       </c>
-      <c r="N22">
+      <c r="P22">
         <v>0.2</v>
       </c>
-      <c r="O22">
+      <c r="R22">
         <v>6</v>
       </c>
-      <c r="P22">
+      <c r="S22">
         <v>220</v>
       </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-      <c r="R22">
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
         <v>-1</v>
       </c>
-      <c r="S22">
+      <c r="V22">
         <v>0.4</v>
       </c>
-      <c r="T22">
+      <c r="X22">
         <v>10</v>
       </c>
-      <c r="U22">
+      <c r="Y22">
         <v>150</v>
       </c>
-      <c r="V22">
-        <v>0</v>
-      </c>
-      <c r="W22">
+      <c r="Z22">
+        <v>0</v>
+      </c>
+      <c r="AA22">
         <v>2</v>
       </c>
-      <c r="X22">
+      <c r="AB22">
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>20</v>
       </c>
@@ -2200,68 +2214,68 @@
       <c r="D23">
         <v>29</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>20</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>340</v>
       </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
         <v>0.1</v>
       </c>
-      <c r="J23">
+      <c r="L23">
         <v>18</v>
       </c>
-      <c r="K23">
+      <c r="M23">
         <v>420</v>
       </c>
-      <c r="L23">
+      <c r="N23">
         <v>-1</v>
       </c>
-      <c r="M23">
+      <c r="O23">
         <v>-1</v>
       </c>
-      <c r="N23">
+      <c r="P23">
         <v>0.2</v>
       </c>
-      <c r="O23">
+      <c r="R23">
         <v>16</v>
       </c>
-      <c r="P23">
+      <c r="S23">
         <v>480</v>
       </c>
-      <c r="Q23">
+      <c r="T23">
         <v>-2</v>
       </c>
-      <c r="R23">
+      <c r="U23">
         <v>-2</v>
       </c>
-      <c r="S23">
+      <c r="V23">
         <v>0.4</v>
       </c>
-      <c r="T23">
+      <c r="X23">
         <v>22</v>
       </c>
-      <c r="U23">
+      <c r="Y23">
         <v>350</v>
       </c>
-      <c r="V23">
+      <c r="Z23">
         <v>2</v>
       </c>
-      <c r="W23">
+      <c r="AA23">
         <v>1</v>
       </c>
-      <c r="X23">
+      <c r="AB23">
         <v>0.01</v>
       </c>
     </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>21</v>
       </c>
@@ -2271,68 +2285,68 @@
       <c r="D24">
         <v>25</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>4</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>60</v>
       </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
         <v>0.1</v>
       </c>
-      <c r="J24">
+      <c r="L24">
         <v>3</v>
       </c>
-      <c r="K24">
+      <c r="M24">
         <v>90</v>
       </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
         <v>-1</v>
       </c>
-      <c r="N24">
+      <c r="P24">
         <v>0.2</v>
       </c>
-      <c r="O24">
+      <c r="R24">
         <v>2</v>
       </c>
-      <c r="P24">
+      <c r="S24">
         <v>130</v>
       </c>
-      <c r="Q24">
-        <v>0</v>
-      </c>
-      <c r="R24">
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
         <v>-1</v>
       </c>
-      <c r="S24">
+      <c r="V24">
         <v>0.4</v>
       </c>
-      <c r="T24">
+      <c r="X24">
         <v>6</v>
       </c>
-      <c r="U24">
+      <c r="Y24">
         <v>70</v>
       </c>
-      <c r="V24">
-        <v>0</v>
-      </c>
-      <c r="W24">
+      <c r="Z24">
+        <v>0</v>
+      </c>
+      <c r="AA24">
         <v>2</v>
       </c>
-      <c r="X24">
+      <c r="AB24">
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>22</v>
       </c>
@@ -2342,68 +2356,68 @@
       <c r="D25">
         <v>31</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>15</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>180</v>
       </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
       <c r="H25">
         <v>0</v>
       </c>
       <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
         <v>0.1</v>
       </c>
-      <c r="J25">
+      <c r="L25">
         <v>14</v>
       </c>
-      <c r="K25">
-        <v>200</v>
-      </c>
-      <c r="L25">
+      <c r="M25">
+        <v>200</v>
+      </c>
+      <c r="N25">
         <v>-2</v>
       </c>
-      <c r="M25">
+      <c r="O25">
         <v>-2</v>
       </c>
-      <c r="N25">
+      <c r="P25">
         <v>0.2</v>
       </c>
-      <c r="O25">
+      <c r="R25">
         <v>12</v>
       </c>
-      <c r="P25">
+      <c r="S25">
         <v>270</v>
       </c>
-      <c r="Q25">
+      <c r="T25">
         <v>-3</v>
       </c>
-      <c r="R25">
+      <c r="U25">
         <v>-3</v>
       </c>
-      <c r="S25">
+      <c r="V25">
         <v>0.4</v>
       </c>
-      <c r="T25">
+      <c r="X25">
         <v>17</v>
       </c>
-      <c r="U25">
-        <v>200</v>
-      </c>
-      <c r="V25">
+      <c r="Y25">
+        <v>200</v>
+      </c>
+      <c r="Z25">
         <v>2</v>
       </c>
-      <c r="W25">
+      <c r="AA25">
         <v>2</v>
       </c>
-      <c r="X25">
+      <c r="AB25">
         <v>0.01</v>
       </c>
     </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>23</v>
       </c>
@@ -2413,68 +2427,68 @@
       <c r="D26">
         <v>32</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>16</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>600</v>
       </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
       <c r="H26">
         <v>0</v>
       </c>
       <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
         <v>0.1</v>
       </c>
-      <c r="J26">
+      <c r="L26">
         <v>14</v>
       </c>
-      <c r="K26">
+      <c r="M26">
         <v>690</v>
       </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="M26">
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
         <v>-1</v>
       </c>
-      <c r="N26">
+      <c r="P26">
         <v>0.2</v>
       </c>
-      <c r="O26">
+      <c r="R26">
         <v>11</v>
       </c>
-      <c r="P26">
+      <c r="S26">
         <v>790</v>
       </c>
-      <c r="Q26">
-        <v>0</v>
-      </c>
-      <c r="R26">
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
         <v>-2</v>
       </c>
-      <c r="S26">
+      <c r="V26">
         <v>0.4</v>
       </c>
-      <c r="T26">
+      <c r="X26">
         <v>19</v>
       </c>
-      <c r="U26">
+      <c r="Y26">
         <v>620</v>
       </c>
-      <c r="V26">
-        <v>0</v>
-      </c>
-      <c r="W26">
+      <c r="Z26">
+        <v>0</v>
+      </c>
+      <c r="AA26">
         <v>2</v>
       </c>
-      <c r="X26">
+      <c r="AB26">
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>24</v>
       </c>
@@ -2484,68 +2498,68 @@
       <c r="D27">
         <v>26</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>8</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>290</v>
       </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
       <c r="H27">
         <v>0</v>
       </c>
       <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
         <v>0.1</v>
       </c>
-      <c r="J27">
+      <c r="L27">
         <v>7</v>
       </c>
-      <c r="K27">
+      <c r="M27">
         <v>360</v>
       </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27">
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
         <v>-1</v>
       </c>
-      <c r="N27">
+      <c r="P27">
         <v>0.2</v>
       </c>
-      <c r="O27">
+      <c r="R27">
         <v>5</v>
       </c>
-      <c r="P27">
+      <c r="S27">
         <v>490</v>
       </c>
-      <c r="Q27">
-        <v>0</v>
-      </c>
-      <c r="R27">
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
         <v>-2</v>
       </c>
-      <c r="S27">
+      <c r="V27">
         <v>0.4</v>
       </c>
-      <c r="T27">
+      <c r="X27">
         <v>10</v>
       </c>
-      <c r="U27">
+      <c r="Y27">
         <v>300</v>
       </c>
-      <c r="V27">
-        <v>0</v>
-      </c>
-      <c r="W27">
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
         <v>1</v>
       </c>
-      <c r="X27">
+      <c r="AB27">
         <v>0.01</v>
       </c>
     </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>25</v>
       </c>
@@ -2555,68 +2569,68 @@
       <c r="D28">
         <v>30</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>3</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>20</v>
       </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
       <c r="H28">
         <v>0</v>
       </c>
       <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
         <v>0.1</v>
       </c>
-      <c r="J28">
+      <c r="L28">
         <v>2</v>
       </c>
-      <c r="K28">
+      <c r="M28">
         <v>30</v>
       </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
       <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
         <v>0.2</v>
       </c>
-      <c r="O28">
+      <c r="R28">
         <v>1</v>
       </c>
-      <c r="P28">
+      <c r="S28">
         <v>50</v>
       </c>
-      <c r="Q28">
-        <v>0</v>
-      </c>
-      <c r="R28">
-        <v>0</v>
-      </c>
-      <c r="S28">
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
         <v>0.4</v>
       </c>
-      <c r="T28">
+      <c r="X28">
         <v>5</v>
       </c>
-      <c r="U28">
+      <c r="Y28">
         <v>20</v>
       </c>
-      <c r="V28">
-        <v>0</v>
-      </c>
-      <c r="W28">
-        <v>0</v>
-      </c>
-      <c r="X28">
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <v>0</v>
+      </c>
+      <c r="AB28">
         <v>0.01</v>
       </c>
     </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B29">
         <v>26</v>
       </c>
@@ -2626,68 +2640,68 @@
       <c r="D29" t="s">
         <v>63</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>14</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>280</v>
       </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
       <c r="H29">
         <v>0</v>
       </c>
       <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
         <v>0.1</v>
       </c>
-      <c r="J29">
+      <c r="L29">
         <v>12</v>
       </c>
-      <c r="K29">
+      <c r="M29">
         <v>380</v>
       </c>
-      <c r="L29">
+      <c r="N29">
         <v>-1</v>
       </c>
-      <c r="M29">
+      <c r="O29">
         <v>-1</v>
       </c>
-      <c r="N29">
+      <c r="P29">
         <v>0.2</v>
       </c>
-      <c r="O29">
+      <c r="R29">
         <v>10</v>
       </c>
-      <c r="P29">
+      <c r="S29">
         <v>470</v>
       </c>
-      <c r="Q29">
+      <c r="T29">
         <v>-2</v>
       </c>
-      <c r="R29">
+      <c r="U29">
         <v>-2</v>
       </c>
-      <c r="S29">
+      <c r="V29">
         <v>0.4</v>
       </c>
-      <c r="T29">
+      <c r="X29">
         <v>16</v>
       </c>
-      <c r="U29">
+      <c r="Y29">
         <v>290</v>
       </c>
-      <c r="V29">
+      <c r="Z29">
         <v>2</v>
       </c>
-      <c r="W29">
+      <c r="AA29">
         <v>2</v>
       </c>
-      <c r="X29">
+      <c r="AB29">
         <v>0.01</v>
       </c>
     </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B30">
         <v>27</v>
       </c>
@@ -2697,68 +2711,68 @@
       <c r="D30" t="s">
         <v>63</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>9</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>60</v>
       </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
       <c r="H30">
         <v>0</v>
       </c>
       <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
         <v>0.1</v>
       </c>
-      <c r="J30">
+      <c r="L30">
         <v>8</v>
       </c>
-      <c r="K30">
+      <c r="M30">
         <v>90</v>
       </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
-      <c r="M30">
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
         <v>-1</v>
       </c>
-      <c r="N30">
+      <c r="P30">
         <v>0.2</v>
       </c>
-      <c r="O30">
+      <c r="R30">
         <v>7</v>
       </c>
-      <c r="P30">
+      <c r="S30">
         <v>130</v>
       </c>
-      <c r="Q30">
-        <v>0</v>
-      </c>
-      <c r="R30">
+      <c r="T30">
+        <v>0</v>
+      </c>
+      <c r="U30">
         <v>-2</v>
       </c>
-      <c r="S30">
+      <c r="V30">
         <v>0.4</v>
       </c>
-      <c r="T30">
+      <c r="X30">
         <v>10</v>
       </c>
-      <c r="U30">
+      <c r="Y30">
         <v>60</v>
       </c>
-      <c r="V30">
-        <v>0</v>
-      </c>
-      <c r="W30">
+      <c r="Z30">
+        <v>0</v>
+      </c>
+      <c r="AA30">
         <v>1</v>
       </c>
-      <c r="X30">
+      <c r="AB30">
         <v>0.01</v>
       </c>
     </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B31">
         <v>28</v>
       </c>
@@ -2768,68 +2782,68 @@
       <c r="D31" t="s">
         <v>63</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>7</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>50</v>
       </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
       <c r="H31">
         <v>0</v>
       </c>
       <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
         <v>0.1</v>
       </c>
-      <c r="J31">
+      <c r="L31">
         <v>6</v>
       </c>
-      <c r="K31">
+      <c r="M31">
         <v>70</v>
       </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-      <c r="M31">
-        <v>0</v>
-      </c>
       <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
         <v>0.2</v>
       </c>
-      <c r="O31">
+      <c r="R31">
         <v>5</v>
       </c>
-      <c r="P31">
+      <c r="S31">
         <v>80</v>
       </c>
-      <c r="Q31">
-        <v>0</v>
-      </c>
-      <c r="R31">
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
         <v>-1</v>
       </c>
-      <c r="S31">
+      <c r="V31">
         <v>0.4</v>
       </c>
-      <c r="T31">
+      <c r="X31">
         <v>9</v>
       </c>
-      <c r="U31">
+      <c r="Y31">
         <v>50</v>
       </c>
-      <c r="V31">
-        <v>0</v>
-      </c>
-      <c r="W31">
+      <c r="Z31">
+        <v>0</v>
+      </c>
+      <c r="AA31">
         <v>1</v>
       </c>
-      <c r="X31">
+      <c r="AB31">
         <v>0.01</v>
       </c>
     </row>
-    <row r="32" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>29</v>
       </c>
@@ -2839,68 +2853,68 @@
       <c r="D32" t="s">
         <v>63</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>8</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>40</v>
       </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
       <c r="H32">
         <v>0</v>
       </c>
       <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
         <v>0.1</v>
       </c>
-      <c r="J32">
+      <c r="L32">
         <v>7</v>
       </c>
-      <c r="K32">
+      <c r="M32">
         <v>60</v>
       </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
-      <c r="M32">
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
         <v>-1</v>
       </c>
-      <c r="N32">
+      <c r="P32">
         <v>0.2</v>
       </c>
-      <c r="O32">
+      <c r="R32">
         <v>5</v>
       </c>
-      <c r="P32">
+      <c r="S32">
         <v>110</v>
       </c>
-      <c r="Q32">
-        <v>0</v>
-      </c>
-      <c r="R32">
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32">
         <v>-2</v>
       </c>
-      <c r="S32">
+      <c r="V32">
         <v>0.4</v>
       </c>
-      <c r="T32">
+      <c r="X32">
         <v>10</v>
       </c>
-      <c r="U32">
+      <c r="Y32">
         <v>50</v>
       </c>
-      <c r="V32">
-        <v>0</v>
-      </c>
-      <c r="W32">
+      <c r="Z32">
+        <v>0</v>
+      </c>
+      <c r="AA32">
         <v>2</v>
       </c>
-      <c r="X32">
+      <c r="AB32">
         <v>0.01</v>
       </c>
     </row>
-    <row r="33" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B33">
         <v>30</v>
       </c>
@@ -2910,68 +2924,68 @@
       <c r="D33" t="s">
         <v>63</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>2</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>30</v>
       </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
       <c r="H33">
         <v>0</v>
       </c>
       <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
         <v>0.1</v>
       </c>
-      <c r="J33">
+      <c r="L33">
         <v>2</v>
       </c>
-      <c r="K33">
+      <c r="M33">
         <v>20</v>
       </c>
-      <c r="L33">
-        <v>0</v>
-      </c>
-      <c r="M33">
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
         <v>-1</v>
       </c>
-      <c r="N33">
+      <c r="P33">
         <v>0.2</v>
       </c>
-      <c r="O33">
+      <c r="R33">
         <v>1</v>
       </c>
-      <c r="P33">
+      <c r="S33">
         <v>50</v>
       </c>
-      <c r="Q33">
-        <v>0</v>
-      </c>
-      <c r="R33">
-        <v>0</v>
-      </c>
-      <c r="S33">
+      <c r="T33">
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="V33">
         <v>0.4</v>
       </c>
-      <c r="T33">
+      <c r="X33">
         <v>4</v>
       </c>
-      <c r="U33">
+      <c r="Y33">
         <v>30</v>
       </c>
-      <c r="V33">
-        <v>0</v>
-      </c>
-      <c r="W33">
+      <c r="Z33">
+        <v>0</v>
+      </c>
+      <c r="AA33">
         <v>2</v>
       </c>
-      <c r="X33">
+      <c r="AB33">
         <v>0.01</v>
       </c>
     </row>
-    <row r="34" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B34">
         <v>31</v>
       </c>
@@ -2981,68 +2995,68 @@
       <c r="D34" t="s">
         <v>63</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>10</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>140</v>
       </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
       <c r="H34">
         <v>0</v>
       </c>
       <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
         <v>0.1</v>
       </c>
-      <c r="J34">
+      <c r="L34">
         <v>9</v>
       </c>
-      <c r="K34">
+      <c r="M34">
         <v>190</v>
       </c>
-      <c r="L34">
+      <c r="N34">
         <v>-2</v>
       </c>
-      <c r="M34">
+      <c r="O34">
         <v>-1</v>
       </c>
-      <c r="N34">
+      <c r="P34">
         <v>0.2</v>
       </c>
-      <c r="O34">
+      <c r="R34">
         <v>7</v>
       </c>
-      <c r="P34">
+      <c r="S34">
         <v>220</v>
       </c>
-      <c r="Q34">
+      <c r="T34">
         <v>-3</v>
       </c>
-      <c r="R34">
+      <c r="U34">
         <v>-1</v>
       </c>
-      <c r="S34">
+      <c r="V34">
         <v>0.4</v>
       </c>
-      <c r="T34">
+      <c r="X34">
         <v>12</v>
       </c>
-      <c r="U34">
+      <c r="Y34">
         <v>150</v>
       </c>
-      <c r="V34">
+      <c r="Z34">
         <v>2</v>
       </c>
-      <c r="W34">
+      <c r="AA34">
         <v>1</v>
       </c>
-      <c r="X34">
+      <c r="AB34">
         <v>0.01</v>
       </c>
     </row>
-    <row r="35" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B35">
         <v>32</v>
       </c>
@@ -3052,68 +3066,68 @@
       <c r="D35" t="s">
         <v>63</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>6</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>340</v>
       </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
       <c r="H35">
         <v>0</v>
       </c>
       <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
         <v>0.1</v>
       </c>
-      <c r="J35">
+      <c r="L35">
         <v>5</v>
       </c>
-      <c r="K35">
+      <c r="M35">
         <v>370</v>
       </c>
-      <c r="L35">
-        <v>0</v>
-      </c>
-      <c r="M35">
-        <v>0</v>
-      </c>
       <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
         <v>0.2</v>
       </c>
-      <c r="O35">
+      <c r="R35">
         <v>4</v>
       </c>
-      <c r="P35">
+      <c r="S35">
         <v>410</v>
       </c>
-      <c r="Q35">
-        <v>0</v>
-      </c>
-      <c r="R35">
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35">
         <v>-2</v>
       </c>
-      <c r="S35">
+      <c r="V35">
         <v>0.4</v>
       </c>
-      <c r="T35">
+      <c r="X35">
         <v>8</v>
       </c>
-      <c r="U35">
+      <c r="Y35">
         <v>360</v>
       </c>
-      <c r="V35">
-        <v>0</v>
-      </c>
-      <c r="W35">
+      <c r="Z35">
+        <v>0</v>
+      </c>
+      <c r="AA35">
         <v>2</v>
       </c>
-      <c r="X35">
+      <c r="AB35">
         <v>0.01</v>
       </c>
     </row>
-    <row r="36" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B36">
         <v>33</v>
       </c>
@@ -3123,68 +3137,68 @@
       <c r="D36" t="s">
         <v>62</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>3</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>110</v>
       </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
       <c r="H36">
         <v>0</v>
       </c>
       <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
         <v>0.1</v>
       </c>
-      <c r="J36">
+      <c r="L36">
         <v>2</v>
       </c>
-      <c r="K36">
+      <c r="M36">
         <v>160</v>
       </c>
-      <c r="L36">
+      <c r="N36">
         <v>-1</v>
       </c>
-      <c r="M36">
+      <c r="O36">
         <v>-1</v>
       </c>
-      <c r="N36">
+      <c r="P36">
         <v>0.2</v>
       </c>
-      <c r="O36">
+      <c r="R36">
         <v>1</v>
       </c>
-      <c r="P36">
-        <v>200</v>
-      </c>
-      <c r="Q36">
+      <c r="S36">
+        <v>200</v>
+      </c>
+      <c r="T36">
         <v>-2</v>
       </c>
-      <c r="R36">
+      <c r="U36">
         <v>-2</v>
       </c>
-      <c r="S36">
+      <c r="V36">
         <v>0.4</v>
       </c>
-      <c r="T36">
+      <c r="X36">
         <v>5</v>
       </c>
-      <c r="U36">
-        <v>120</v>
-      </c>
-      <c r="V36">
+      <c r="Y36">
+        <v>120</v>
+      </c>
+      <c r="Z36">
         <v>2</v>
       </c>
-      <c r="W36">
+      <c r="AA36">
         <v>2</v>
       </c>
-      <c r="X36">
+      <c r="AB36">
         <v>0.01</v>
       </c>
     </row>
-    <row r="37" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B37">
         <v>34</v>
       </c>
@@ -3194,68 +3208,68 @@
       <c r="D37">
         <v>37</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>4</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>80</v>
       </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
       <c r="H37">
         <v>0</v>
       </c>
       <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
         <v>0.1</v>
       </c>
-      <c r="J37">
+      <c r="L37">
         <v>3</v>
       </c>
-      <c r="K37">
+      <c r="M37">
         <v>90</v>
       </c>
-      <c r="L37">
-        <v>0</v>
-      </c>
-      <c r="M37">
-        <v>0</v>
-      </c>
       <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
         <v>0.2</v>
       </c>
-      <c r="O37">
+      <c r="R37">
         <v>2</v>
       </c>
-      <c r="P37">
+      <c r="S37">
         <v>130</v>
       </c>
-      <c r="Q37">
+      <c r="T37">
         <v>-1</v>
       </c>
-      <c r="R37">
+      <c r="U37">
         <v>-1</v>
       </c>
-      <c r="S37">
+      <c r="V37">
         <v>0.4</v>
       </c>
-      <c r="T37">
+      <c r="X37">
         <v>5</v>
       </c>
-      <c r="U37">
+      <c r="Y37">
         <v>90</v>
       </c>
-      <c r="V37">
+      <c r="Z37">
         <v>1</v>
       </c>
-      <c r="W37">
+      <c r="AA37">
         <v>1</v>
       </c>
-      <c r="X37">
+      <c r="AB37">
         <v>0.01</v>
       </c>
     </row>
-    <row r="38" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B38">
         <v>35</v>
       </c>
@@ -3265,68 +3279,68 @@
       <c r="D38">
         <v>38</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>5</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>210</v>
       </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
       <c r="H38">
         <v>0</v>
       </c>
       <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
         <v>0.1</v>
       </c>
-      <c r="J38">
+      <c r="L38">
         <v>4</v>
       </c>
-      <c r="K38">
+      <c r="M38">
         <v>240</v>
       </c>
-      <c r="L38">
-        <v>0</v>
-      </c>
-      <c r="M38">
-        <v>0</v>
-      </c>
       <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
         <v>0.2</v>
       </c>
-      <c r="O38">
+      <c r="R38">
         <v>3</v>
       </c>
-      <c r="P38">
+      <c r="S38">
         <v>280</v>
       </c>
-      <c r="Q38">
-        <v>0</v>
-      </c>
-      <c r="R38">
-        <v>0</v>
-      </c>
-      <c r="S38">
+      <c r="T38">
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <v>0</v>
+      </c>
+      <c r="V38">
         <v>0.4</v>
       </c>
-      <c r="T38">
+      <c r="X38">
         <v>6</v>
       </c>
-      <c r="U38">
+      <c r="Y38">
         <v>220</v>
       </c>
-      <c r="V38">
+      <c r="Z38">
         <v>2</v>
       </c>
-      <c r="W38">
+      <c r="AA38">
         <v>1</v>
       </c>
-      <c r="X38">
+      <c r="AB38">
         <v>0.01</v>
       </c>
     </row>
-    <row r="39" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B39">
         <v>36</v>
       </c>
@@ -3336,68 +3350,68 @@
       <c r="D39">
         <v>38</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>3</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>70</v>
       </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
       <c r="H39">
         <v>0</v>
       </c>
       <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
         <v>0.1</v>
       </c>
-      <c r="J39">
+      <c r="L39">
         <v>2</v>
       </c>
-      <c r="K39">
+      <c r="M39">
         <v>80</v>
       </c>
-      <c r="L39">
-        <v>0</v>
-      </c>
-      <c r="M39">
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
         <v>-1</v>
       </c>
-      <c r="N39">
+      <c r="P39">
         <v>0.2</v>
       </c>
-      <c r="O39">
+      <c r="R39">
         <v>1</v>
       </c>
-      <c r="P39">
+      <c r="S39">
         <v>110</v>
       </c>
-      <c r="Q39">
-        <v>0</v>
-      </c>
-      <c r="R39">
+      <c r="T39">
+        <v>0</v>
+      </c>
+      <c r="U39">
         <v>-1</v>
       </c>
-      <c r="S39">
+      <c r="V39">
         <v>0.4</v>
       </c>
-      <c r="T39">
+      <c r="X39">
         <v>4</v>
       </c>
-      <c r="U39">
+      <c r="Y39">
         <v>70</v>
       </c>
-      <c r="V39">
+      <c r="Z39">
         <v>1</v>
       </c>
-      <c r="W39">
+      <c r="AA39">
         <v>2</v>
       </c>
-      <c r="X39">
+      <c r="AB39">
         <v>0.01</v>
       </c>
     </row>
-    <row r="40" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B40">
         <v>37</v>
       </c>
@@ -3407,68 +3421,68 @@
       <c r="D40">
         <v>38</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>3</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>50</v>
       </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
       <c r="H40">
         <v>0</v>
       </c>
       <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
         <v>0.1</v>
       </c>
-      <c r="J40">
+      <c r="L40">
         <v>2</v>
       </c>
-      <c r="K40">
+      <c r="M40">
         <v>60</v>
       </c>
-      <c r="L40">
+      <c r="N40">
         <v>-1</v>
       </c>
-      <c r="M40">
-        <v>0</v>
-      </c>
-      <c r="N40">
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
         <v>0.2</v>
       </c>
-      <c r="O40">
+      <c r="R40">
         <v>1</v>
       </c>
-      <c r="P40">
-        <v>100</v>
-      </c>
-      <c r="Q40">
+      <c r="S40">
+        <v>100</v>
+      </c>
+      <c r="T40">
         <v>-1</v>
       </c>
-      <c r="R40">
-        <v>0</v>
-      </c>
-      <c r="S40">
+      <c r="U40">
+        <v>0</v>
+      </c>
+      <c r="V40">
         <v>0.4</v>
       </c>
-      <c r="T40">
+      <c r="X40">
         <v>4</v>
       </c>
-      <c r="U40">
+      <c r="Y40">
         <v>60</v>
       </c>
-      <c r="V40">
+      <c r="Z40">
         <v>1</v>
       </c>
-      <c r="W40">
-        <v>0</v>
-      </c>
-      <c r="X40">
+      <c r="AA40">
+        <v>0</v>
+      </c>
+      <c r="AB40">
         <v>0.01</v>
       </c>
     </row>
-    <row r="41" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B41">
         <v>38</v>
       </c>
@@ -3478,68 +3492,68 @@
       <c r="D41" t="s">
         <v>64</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>3</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>90</v>
       </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
       <c r="H41">
         <v>0</v>
       </c>
       <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
         <v>0.1</v>
       </c>
-      <c r="J41">
+      <c r="L41">
         <v>2</v>
       </c>
-      <c r="K41">
+      <c r="M41">
         <v>170</v>
       </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-      <c r="M41">
-        <v>0</v>
-      </c>
       <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
         <v>0.2</v>
       </c>
-      <c r="O41">
+      <c r="R41">
         <v>1</v>
       </c>
-      <c r="P41">
+      <c r="S41">
         <v>240</v>
       </c>
-      <c r="Q41">
-        <v>0</v>
-      </c>
-      <c r="R41">
-        <v>0</v>
-      </c>
-      <c r="S41">
+      <c r="T41">
+        <v>0</v>
+      </c>
+      <c r="U41">
+        <v>0</v>
+      </c>
+      <c r="V41">
         <v>0.4</v>
       </c>
-      <c r="T41">
+      <c r="X41">
         <v>4</v>
       </c>
-      <c r="U41">
-        <v>100</v>
-      </c>
-      <c r="V41">
+      <c r="Y41">
+        <v>100</v>
+      </c>
+      <c r="Z41">
         <v>2</v>
       </c>
-      <c r="W41">
+      <c r="AA41">
         <v>1</v>
       </c>
-      <c r="X41">
+      <c r="AB41">
         <v>0.01</v>
       </c>
     </row>
-    <row r="42" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B42">
         <v>39</v>
       </c>
@@ -3549,68 +3563,68 @@
       <c r="D42">
         <v>44</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>3</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>60</v>
       </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
       <c r="H42">
         <v>0</v>
       </c>
       <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
         <v>0.1</v>
       </c>
-      <c r="J42">
+      <c r="L42">
         <v>2</v>
       </c>
-      <c r="K42">
+      <c r="M42">
         <v>90</v>
       </c>
-      <c r="L42">
+      <c r="N42">
         <v>-1</v>
       </c>
-      <c r="M42">
+      <c r="O42">
         <v>-1</v>
       </c>
-      <c r="N42">
+      <c r="P42">
         <v>0.2</v>
       </c>
-      <c r="O42">
+      <c r="R42">
         <v>1</v>
       </c>
-      <c r="P42">
+      <c r="S42">
         <v>160</v>
       </c>
-      <c r="Q42">
+      <c r="T42">
         <v>-2</v>
       </c>
-      <c r="R42">
+      <c r="U42">
         <v>-2</v>
       </c>
-      <c r="S42">
+      <c r="V42">
         <v>0.4</v>
       </c>
-      <c r="T42">
+      <c r="X42">
         <v>5</v>
       </c>
-      <c r="U42">
+      <c r="Y42">
         <v>90</v>
       </c>
-      <c r="V42">
+      <c r="Z42">
         <v>2</v>
       </c>
-      <c r="W42">
+      <c r="AA42">
         <v>2</v>
       </c>
-      <c r="X42">
+      <c r="AB42">
         <v>0.01</v>
       </c>
     </row>
-    <row r="43" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B43">
         <v>40</v>
       </c>
@@ -3620,68 +3634,68 @@
       <c r="D43">
         <v>44</v>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>3</v>
       </c>
-      <c r="F43">
+      <c r="G43">
         <v>45</v>
       </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
       <c r="H43">
         <v>0</v>
       </c>
       <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
         <v>0.1</v>
       </c>
-      <c r="J43">
+      <c r="L43">
         <v>2</v>
       </c>
-      <c r="K43">
+      <c r="M43">
         <v>60</v>
       </c>
-      <c r="L43">
+      <c r="N43">
         <v>-2</v>
       </c>
-      <c r="M43">
+      <c r="O43">
         <v>-1</v>
       </c>
-      <c r="N43">
+      <c r="P43">
         <v>0.2</v>
       </c>
-      <c r="O43">
+      <c r="R43">
         <v>1</v>
       </c>
-      <c r="P43">
+      <c r="S43">
         <v>130</v>
       </c>
-      <c r="Q43">
+      <c r="T43">
         <v>-3</v>
       </c>
-      <c r="R43">
+      <c r="U43">
         <v>-2</v>
       </c>
-      <c r="S43">
+      <c r="V43">
         <v>0.4</v>
       </c>
-      <c r="T43">
+      <c r="X43">
         <v>4</v>
       </c>
-      <c r="U43">
+      <c r="Y43">
         <v>60</v>
       </c>
-      <c r="V43">
+      <c r="Z43">
         <v>2</v>
       </c>
-      <c r="W43">
+      <c r="AA43">
         <v>1</v>
       </c>
-      <c r="X43">
+      <c r="AB43">
         <v>0.01</v>
       </c>
     </row>
-    <row r="44" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B44">
         <v>41</v>
       </c>
@@ -3691,68 +3705,68 @@
       <c r="D44">
         <v>44</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>4</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>65</v>
       </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
       <c r="H44">
         <v>0</v>
       </c>
       <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
         <v>0.1</v>
       </c>
-      <c r="J44">
+      <c r="L44">
         <v>3</v>
       </c>
-      <c r="K44">
+      <c r="M44">
         <v>70</v>
       </c>
-      <c r="L44">
-        <v>0</v>
-      </c>
-      <c r="M44">
-        <v>0</v>
-      </c>
       <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
         <v>0.2</v>
       </c>
-      <c r="O44">
+      <c r="R44">
         <v>2</v>
       </c>
-      <c r="P44">
+      <c r="S44">
         <v>110</v>
       </c>
-      <c r="Q44">
-        <v>0</v>
-      </c>
-      <c r="R44">
-        <v>0</v>
-      </c>
-      <c r="S44">
+      <c r="T44">
+        <v>0</v>
+      </c>
+      <c r="U44">
+        <v>0</v>
+      </c>
+      <c r="V44">
         <v>0.4</v>
       </c>
-      <c r="T44">
+      <c r="X44">
         <v>5</v>
       </c>
-      <c r="U44">
+      <c r="Y44">
         <v>60</v>
       </c>
-      <c r="V44">
+      <c r="Z44">
         <v>1</v>
       </c>
-      <c r="W44">
+      <c r="AA44">
         <v>1</v>
       </c>
-      <c r="X44">
+      <c r="AB44">
         <v>0.01</v>
       </c>
     </row>
-    <row r="45" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B45">
         <v>42</v>
       </c>
@@ -3762,68 +3776,68 @@
       <c r="D45" t="s">
         <v>65</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>3</v>
       </c>
-      <c r="F45">
+      <c r="G45">
         <v>50</v>
       </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
       <c r="H45">
         <v>0</v>
       </c>
       <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
         <v>0.1</v>
       </c>
-      <c r="J45">
+      <c r="L45">
         <v>2</v>
       </c>
-      <c r="K45">
+      <c r="M45">
         <v>90</v>
       </c>
-      <c r="L45">
-        <v>0</v>
-      </c>
-      <c r="M45">
-        <v>0</v>
-      </c>
       <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
         <v>0.2</v>
       </c>
-      <c r="O45">
+      <c r="R45">
         <v>1</v>
       </c>
-      <c r="P45">
-        <v>120</v>
-      </c>
-      <c r="Q45">
-        <v>0</v>
-      </c>
-      <c r="R45">
-        <v>0</v>
-      </c>
       <c r="S45">
+        <v>120</v>
+      </c>
+      <c r="T45">
+        <v>0</v>
+      </c>
+      <c r="U45">
+        <v>0</v>
+      </c>
+      <c r="V45">
         <v>0.4</v>
       </c>
-      <c r="T45">
+      <c r="X45">
         <v>4</v>
       </c>
-      <c r="U45">
+      <c r="Y45">
         <v>50</v>
       </c>
-      <c r="V45">
-        <v>0</v>
-      </c>
-      <c r="W45">
-        <v>0</v>
-      </c>
-      <c r="X45">
+      <c r="Z45">
+        <v>0</v>
+      </c>
+      <c r="AA45">
+        <v>0</v>
+      </c>
+      <c r="AB45">
         <v>0.01</v>
       </c>
     </row>
-    <row r="46" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B46">
         <v>43</v>
       </c>
@@ -3833,68 +3847,68 @@
       <c r="D46">
         <v>46</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>3</v>
       </c>
-      <c r="F46">
+      <c r="G46">
         <v>70</v>
       </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
       <c r="H46">
         <v>0</v>
       </c>
       <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
         <v>0.1</v>
       </c>
-      <c r="J46">
+      <c r="L46">
         <v>2</v>
       </c>
-      <c r="K46">
-        <v>100</v>
-      </c>
-      <c r="L46">
-        <v>0</v>
-      </c>
       <c r="M46">
+        <v>100</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
         <v>-1</v>
       </c>
-      <c r="N46">
+      <c r="P46">
         <v>0.2</v>
       </c>
-      <c r="O46">
+      <c r="R46">
         <v>1</v>
       </c>
-      <c r="P46">
+      <c r="S46">
         <v>140</v>
       </c>
-      <c r="Q46">
-        <v>0</v>
-      </c>
-      <c r="R46">
+      <c r="T46">
+        <v>0</v>
+      </c>
+      <c r="U46">
         <v>-2</v>
       </c>
-      <c r="S46">
+      <c r="V46">
         <v>0.4</v>
       </c>
-      <c r="T46">
+      <c r="X46">
         <v>5</v>
       </c>
-      <c r="U46">
+      <c r="Y46">
         <v>60</v>
       </c>
-      <c r="V46">
-        <v>0</v>
-      </c>
-      <c r="W46">
+      <c r="Z46">
+        <v>0</v>
+      </c>
+      <c r="AA46">
         <v>2</v>
       </c>
-      <c r="X46">
+      <c r="AB46">
         <v>0.01</v>
       </c>
     </row>
-    <row r="47" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B47">
         <v>44</v>
       </c>
@@ -3904,53 +3918,53 @@
       <c r="D47">
         <v>46</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>2</v>
       </c>
-      <c r="F47">
+      <c r="G47">
         <v>35</v>
       </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
       <c r="H47">
         <v>0</v>
       </c>
       <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
         <v>0.1</v>
       </c>
-      <c r="J47">
+      <c r="L47">
         <v>1</v>
       </c>
-      <c r="K47">
+      <c r="M47">
         <v>70</v>
       </c>
-      <c r="L47">
-        <v>0</v>
-      </c>
-      <c r="M47">
-        <v>0</v>
-      </c>
       <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="P47">
         <v>0.2</v>
       </c>
-      <c r="T47">
+      <c r="X47">
         <v>3</v>
       </c>
-      <c r="U47">
+      <c r="Y47">
         <v>30</v>
       </c>
-      <c r="V47">
-        <v>0</v>
-      </c>
-      <c r="W47">
-        <v>0</v>
-      </c>
-      <c r="X47">
+      <c r="Z47">
+        <v>0</v>
+      </c>
+      <c r="AA47">
+        <v>0</v>
+      </c>
+      <c r="AB47">
         <v>0.01</v>
       </c>
     </row>
-    <row r="48" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B48">
         <v>45</v>
       </c>
@@ -3960,87 +3974,87 @@
       <c r="D48">
         <v>46</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>2</v>
       </c>
-      <c r="F48">
+      <c r="G48">
         <v>40</v>
       </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
       <c r="H48">
         <v>0</v>
       </c>
       <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
         <v>0.1</v>
       </c>
-      <c r="J48">
+      <c r="L48">
         <v>1</v>
       </c>
-      <c r="K48">
+      <c r="M48">
         <v>60</v>
       </c>
-      <c r="L48">
-        <v>0</v>
-      </c>
-      <c r="M48">
-        <v>0</v>
-      </c>
       <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+      <c r="P48">
         <v>0.2</v>
       </c>
-      <c r="T48">
+      <c r="X48">
         <v>3</v>
       </c>
-      <c r="U48">
+      <c r="Y48">
         <v>30</v>
       </c>
-      <c r="V48">
-        <v>0</v>
-      </c>
-      <c r="W48">
-        <v>0</v>
-      </c>
-      <c r="X48">
+      <c r="Z48">
+        <v>0</v>
+      </c>
+      <c r="AA48">
+        <v>0</v>
+      </c>
+      <c r="AB48">
         <v>0.01</v>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B49">
         <v>46</v>
       </c>
       <c r="C49" t="s">
         <v>54</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>1</v>
       </c>
-      <c r="F49">
+      <c r="G49">
         <v>30</v>
       </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
       <c r="H49">
         <v>0</v>
       </c>
       <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
         <v>0.1</v>
       </c>
-      <c r="J49">
-        <v>0</v>
-      </c>
-      <c r="K49">
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
         <v>150</v>
       </c>
-      <c r="L49">
-        <v>0</v>
-      </c>
-      <c r="M49">
-        <v>0</v>
-      </c>
       <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="P49">
         <v>0.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
worked on topsim model definition
</commit_message>
<xml_diff>
--- a/Model_TopSim_RollerCoaster/RollerCoaster_Model_Definition.xlsx
+++ b/Model_TopSim_RollerCoaster/RollerCoaster_Model_Definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malteebner/Library/Mobile Documents/com~apple~CloudDocs/Master ETIT/10. Semester/Forschungsarbeit/Code Forschungsarbeit/Model_TopSim_RollerCoaster/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB548049-4167-504E-92D0-EA514D70D6BD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6E4274-6670-374A-9AA9-7E22328315E3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{FCED99B0-49FF-5541-B4A0-4C6030238B64}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680" xr2:uid="{FCED99B0-49FF-5541-B4A0-4C6030238B64}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A15AD41-7732-DC45-B8B2-B8C789AA2988}">
   <dimension ref="A1:AR49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4914,21 +4914,21 @@
         <v>150</v>
       </c>
       <c r="E31">
-        <f t="shared" ref="E29:E47" si="3">E32-D31</f>
+        <f t="shared" ref="E31:E47" si="3">E32-D31</f>
         <v>-4300</v>
       </c>
       <c r="H31">
         <v>100</v>
       </c>
       <c r="I31">
-        <f t="shared" ref="I29:I44" si="4">I32-H31</f>
+        <f t="shared" ref="I31:I44" si="4">I32-H31</f>
         <v>-2120</v>
       </c>
       <c r="L31">
         <v>100</v>
       </c>
       <c r="M31">
-        <f t="shared" ref="M29:M42" si="5">M32-L31</f>
+        <f t="shared" ref="M31:M42" si="5">M32-L31</f>
         <v>-2050</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added graphs for losses to roller coaster model definitions
</commit_message>
<xml_diff>
--- a/Model_TopSim_RollerCoaster/RollerCoaster_Model_Definition.xlsx
+++ b/Model_TopSim_RollerCoaster/RollerCoaster_Model_Definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malteebner/Library/Mobile Documents/com~apple~CloudDocs/Master ETIT/10. Semester/Forschungsarbeit/Code Forschungsarbeit/Model_TopSim_RollerCoaster/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AFC39D-1BE6-E645-9C83-51D27841E422}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02ADA2A-2CB0-5042-AD22-AD3A4D2FFF89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25060" windowHeight="16680" activeTab="2" xr2:uid="{FCED99B0-49FF-5541-B4A0-4C6030238B64}"/>
   </bookViews>
@@ -1119,7 +1119,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>bonus(technology)</a:t>
+              <a:t>bonus (technology index)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1965,6 +1965,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> bonus (quality index)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12775,7 +12800,7 @@
   <dimension ref="B1:O146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O20"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>